<commit_message>
Verifying ward level shape against pres2013 results
</commit_message>
<xml_diff>
--- a/data/old_results/2013_presidential/2013Masvingo_Presidential_Results_Formatted_13-08-2013.xlsx
+++ b/data/old_results/2013_presidential/2013Masvingo_Presidential_Results_Formatted_13-08-2013.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\office\Desktop\DI\Zimbabwe_election\data\old_results\2013_presidential\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{86DC4A91-8F93-4ABC-A19A-27F373CE9D94}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D4912268-9F52-43C3-B085-1AC9A5FF3C8B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="29" r:id="rId3"/>
+    <pivotCache cacheId="56" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -34762,7 +34762,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8BCA655F-FBAC-4132-9E51-202EB0657D36}" name="PivotTable9" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8BCA655F-FBAC-4132-9E51-202EB0657D36}" name="PivotTable9" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField showAll="0">
@@ -35178,7 +35178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393C8ACB-5709-42D4-9069-D5D73A7F1C3F}">
   <dimension ref="A3:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -35289,8 +35289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1239"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A1196" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A1239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>